<commit_message>
Falta arreglar cuando se da una fecha
</commit_message>
<xml_diff>
--- a/data/resume.xlsx
+++ b/data/resume.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>date</t>
   </si>
@@ -237,6 +237,30 @@
   </si>
   <si>
     <t>06/11/2025</t>
+  </si>
+  <si>
+    <t>2025-06-12 19:17:34</t>
+  </si>
+  <si>
+    <t>2025-06-12 19:17:35</t>
+  </si>
+  <si>
+    <t>2025-06-12 19:17:36</t>
+  </si>
+  <si>
+    <t>2025-06-12 19:17:37</t>
+  </si>
+  <si>
+    <t>2025-06-12 19:21:26</t>
+  </si>
+  <si>
+    <t>2025-06-12 19:21:27</t>
+  </si>
+  <si>
+    <t>2025-06-12 19:21:28</t>
+  </si>
+  <si>
+    <t>2025-06-12 19:21:29</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1068,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1831,16 +1855,170 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="1">
         <v>4</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>7</v>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="1">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>